<commit_message>
refactor sprint of cost cli and data structure mostly done
</commit_message>
<xml_diff>
--- a/tests/resources/test_cost_profile_output.xlsx
+++ b/tests/resources/test_cost_profile_output.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -361,27 +361,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>current</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Last</t>
+          <t>last</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Baseline one</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Baseline two</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Baseline three</t>
+          <t>bl_one</t>
         </is>
       </c>
     </row>
@@ -400,12 +390,6 @@
       <c r="D2" t="n">
         <v>15.45</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -422,12 +406,6 @@
       <c r="D3" t="n">
         <v>932.8199999999999</v>
       </c>
-      <c r="E3" t="n">
-        <v>932.8199999999999</v>
-      </c>
-      <c r="F3" t="n">
-        <v>932.8199999999999</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -444,12 +422,6 @@
       <c r="D4" t="n">
         <v>798.1</v>
       </c>
-      <c r="E4" t="n">
-        <v>798.1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>798.1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -466,12 +438,6 @@
       <c r="D5" t="n">
         <v>406.81</v>
       </c>
-      <c r="E5" t="n">
-        <v>406.81</v>
-      </c>
-      <c r="F5" t="n">
-        <v>406.81</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -488,12 +454,6 @@
       <c r="D6" t="n">
         <v>266.2</v>
       </c>
-      <c r="E6" t="n">
-        <v>266.2</v>
-      </c>
-      <c r="F6" t="n">
-        <v>266.2</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -510,12 +470,6 @@
       <c r="D7" t="n">
         <v>411.9</v>
       </c>
-      <c r="E7" t="n">
-        <v>411.9</v>
-      </c>
-      <c r="F7" t="n">
-        <v>411.9</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -532,12 +486,6 @@
       <c r="D8" t="n">
         <v>443.8</v>
       </c>
-      <c r="E8" t="n">
-        <v>443.8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>443.8</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -549,16 +497,10 @@
         <v>1235.95</v>
       </c>
       <c r="C9" t="n">
-        <v>728.78</v>
+        <v>848.6500000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>848.65</v>
-      </c>
-      <c r="E9" t="n">
-        <v>848.65</v>
-      </c>
-      <c r="F9" t="n">
-        <v>848.65</v>
+        <v>848.6500000000001</v>
       </c>
     </row>
     <row r="10">
@@ -571,17 +513,11 @@
         <v>1362.52</v>
       </c>
       <c r="C10" t="n">
-        <v>1047.2</v>
+        <v>1194.22</v>
       </c>
       <c r="D10" t="n">
         <v>1194.22</v>
       </c>
-      <c r="E10" t="n">
-        <v>1194.22</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1194.22</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -593,17 +529,11 @@
         <v>1572.957082855212</v>
       </c>
       <c r="C11" t="n">
-        <v>2440.6</v>
+        <v>2728.757082855212</v>
       </c>
       <c r="D11" t="n">
         <v>2728.757082855212</v>
       </c>
-      <c r="E11" t="n">
-        <v>2728.757082855212</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2728.757082855212</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -615,17 +545,11 @@
         <v>1124.88</v>
       </c>
       <c r="C12" t="n">
-        <v>3315.6</v>
+        <v>3505.88</v>
       </c>
       <c r="D12" t="n">
         <v>3505.88</v>
       </c>
-      <c r="E12" t="n">
-        <v>3505.88</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3505.88</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -637,17 +561,11 @@
         <v>534.5699999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>396.44</v>
+        <v>612.01</v>
       </c>
       <c r="D13" t="n">
         <v>612.01</v>
       </c>
-      <c r="E13" t="n">
-        <v>612.01</v>
-      </c>
-      <c r="F13" t="n">
-        <v>612.01</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -659,17 +577,11 @@
         <v>264.61</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6799999999999999</v>
+        <v>217.61</v>
       </c>
       <c r="D14" t="n">
         <v>217.61</v>
       </c>
-      <c r="E14" t="n">
-        <v>217.61</v>
-      </c>
-      <c r="F14" t="n">
-        <v>217.61</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -681,17 +593,11 @@
         <v>221.47</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>219.97</v>
       </c>
       <c r="D15" t="n">
         <v>219.97</v>
       </c>
-      <c r="E15" t="n">
-        <v>219.97</v>
-      </c>
-      <c r="F15" t="n">
-        <v>219.97</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -703,17 +609,11 @@
         <v>223.66</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>223.06</v>
       </c>
       <c r="D16" t="n">
         <v>223.06</v>
       </c>
-      <c r="E16" t="n">
-        <v>223.06</v>
-      </c>
-      <c r="F16" t="n">
-        <v>223.06</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -725,17 +625,11 @@
         <v>226.79</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>226.19</v>
       </c>
       <c r="D17" t="n">
         <v>226.19</v>
       </c>
-      <c r="E17" t="n">
-        <v>226.19</v>
-      </c>
-      <c r="F17" t="n">
-        <v>226.19</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -747,17 +641,11 @@
         <v>229.96</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>229.36</v>
       </c>
       <c r="D18" t="n">
         <v>229.36</v>
       </c>
-      <c r="E18" t="n">
-        <v>229.36</v>
-      </c>
-      <c r="F18" t="n">
-        <v>229.36</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -769,17 +657,11 @@
         <v>233.24</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>232.56</v>
       </c>
       <c r="D19" t="n">
         <v>232.56</v>
       </c>
-      <c r="E19" t="n">
-        <v>232.56</v>
-      </c>
-      <c r="F19" t="n">
-        <v>232.56</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -791,17 +673,11 @@
         <v>217.3</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>216.62</v>
       </c>
       <c r="D20" t="n">
         <v>216.62</v>
       </c>
-      <c r="E20" t="n">
-        <v>216.62</v>
-      </c>
-      <c r="F20" t="n">
-        <v>216.62</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -813,17 +689,11 @@
         <v>145.94</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>145.26</v>
       </c>
       <c r="D21" t="n">
         <v>145.26</v>
       </c>
-      <c r="E21" t="n">
-        <v>145.26</v>
-      </c>
-      <c r="F21" t="n">
-        <v>145.26</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -835,17 +705,11 @@
         <v>51.87</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>51.19</v>
       </c>
       <c r="D22" t="n">
         <v>51.19</v>
       </c>
-      <c r="E22" t="n">
-        <v>51.19</v>
-      </c>
-      <c r="F22" t="n">
-        <v>51.19</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -862,12 +726,6 @@
       <c r="D23" t="n">
         <v>0</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -884,12 +742,6 @@
       <c r="D24" t="n">
         <v>0</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -904,12 +756,6 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactoring tests to use pickle master file. half way
</commit_message>
<xml_diff>
--- a/tests/resources/test_cost_profile_output.xlsx
+++ b/tests/resources/test_cost_profile_output.xlsx
@@ -420,7 +420,7 @@
         <v>798.1</v>
       </c>
       <c r="D4" t="n">
-        <v>798.1</v>
+        <v>757.15</v>
       </c>
     </row>
     <row r="5">
@@ -430,13 +430,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>406.81</v>
+        <v>529.374</v>
       </c>
       <c r="C5" t="n">
-        <v>406.81</v>
+        <v>545.8699999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>406.81</v>
+        <v>545.51</v>
       </c>
     </row>
     <row r="6">
@@ -449,10 +449,10 @@
         <v>362.8</v>
       </c>
       <c r="C6" t="n">
-        <v>266.2</v>
+        <v>338.7</v>
       </c>
       <c r="D6" t="n">
-        <v>266.2</v>
+        <v>306.6</v>
       </c>
     </row>
     <row r="7">
@@ -465,10 +465,10 @@
         <v>344.97</v>
       </c>
       <c r="C7" t="n">
-        <v>411.9</v>
+        <v>432.4</v>
       </c>
       <c r="D7" t="n">
-        <v>411.9</v>
+        <v>426.2</v>
       </c>
     </row>
     <row r="8">
@@ -484,7 +484,7 @@
         <v>443.8</v>
       </c>
       <c r="D8" t="n">
-        <v>443.8</v>
+        <v>443.2</v>
       </c>
     </row>
     <row r="9">
@@ -497,10 +497,10 @@
         <v>1235.95</v>
       </c>
       <c r="C9" t="n">
-        <v>848.6500000000001</v>
+        <v>747.788</v>
       </c>
       <c r="D9" t="n">
-        <v>848.6500000000001</v>
+        <v>747.1080000000001</v>
       </c>
     </row>
     <row r="10">
@@ -513,10 +513,10 @@
         <v>1362.52</v>
       </c>
       <c r="C10" t="n">
-        <v>1194.22</v>
+        <v>1157.636</v>
       </c>
       <c r="D10" t="n">
-        <v>1194.22</v>
+        <v>1157.036</v>
       </c>
     </row>
     <row r="11">
@@ -529,10 +529,10 @@
         <v>1572.957082855212</v>
       </c>
       <c r="C11" t="n">
-        <v>2728.757082855212</v>
+        <v>1652.044</v>
       </c>
       <c r="D11" t="n">
-        <v>2728.757082855212</v>
+        <v>1651.444</v>
       </c>
     </row>
     <row r="12">
@@ -545,10 +545,10 @@
         <v>1124.88</v>
       </c>
       <c r="C12" t="n">
-        <v>3505.88</v>
+        <v>1565.2</v>
       </c>
       <c r="D12" t="n">
-        <v>3505.88</v>
+        <v>1564.6</v>
       </c>
     </row>
     <row r="13">
@@ -561,10 +561,10 @@
         <v>534.5699999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>612.01</v>
+        <v>649.7239999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>612.01</v>
+        <v>649.124</v>
       </c>
     </row>
     <row r="14">
@@ -577,10 +577,10 @@
         <v>264.61</v>
       </c>
       <c r="C14" t="n">
-        <v>217.61</v>
+        <v>257.732</v>
       </c>
       <c r="D14" t="n">
-        <v>217.61</v>
+        <v>257.052</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>221.47</v>
       </c>
       <c r="C15" t="n">
-        <v>219.97</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>219.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -609,10 +609,10 @@
         <v>223.66</v>
       </c>
       <c r="C16" t="n">
-        <v>223.06</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>223.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -625,10 +625,10 @@
         <v>226.79</v>
       </c>
       <c r="C17" t="n">
-        <v>226.19</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>226.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -641,10 +641,10 @@
         <v>229.96</v>
       </c>
       <c r="C18" t="n">
-        <v>229.36</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>229.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -657,10 +657,10 @@
         <v>233.24</v>
       </c>
       <c r="C19" t="n">
-        <v>232.56</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>232.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -673,10 +673,10 @@
         <v>217.3</v>
       </c>
       <c r="C20" t="n">
-        <v>216.62</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>216.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -689,10 +689,10 @@
         <v>145.94</v>
       </c>
       <c r="C21" t="n">
-        <v>145.26</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>145.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -705,10 +705,10 @@
         <v>51.87</v>
       </c>
       <c r="C22" t="n">
-        <v>51.19</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>51.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
central resource data analysis for top250. tweak to how milestones are concatenated in both excel and mpl graphs
</commit_message>
<xml_diff>
--- a/tests/resources/test_cost_profile_output.xlsx
+++ b/tests/resources/test_cost_profile_output.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>15.45</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>15.45</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="3">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>932.8199999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>932.8199999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>932.8199999999999</v>
       </c>
     </row>
     <row r="4">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>798.1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>798.1</v>
       </c>
       <c r="D4" t="n">
-        <v>695.25</v>
+        <v>757.15</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
algorithm added to distribute group circles. Nolonger hard coded
</commit_message>
<xml_diff>
--- a/tests/resources/test_cost_profile_output.xlsx
+++ b/tests/resources/test_cost_profile_output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,219 +446,219 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16-17</t>
+          <t>21-22</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15.45</v>
+        <v>344.97</v>
       </c>
       <c r="C2" t="n">
-        <v>15.45</v>
+        <v>432.4</v>
       </c>
       <c r="D2" t="n">
-        <v>15.45</v>
+        <v>426.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17-18</t>
+          <t>22-23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>932.8199999999999</v>
+        <v>943.0700000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>932.8199999999999</v>
+        <v>443.8</v>
       </c>
       <c r="D3" t="n">
-        <v>932.8199999999999</v>
+        <v>443.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18-19</t>
+          <t>23-24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>798.1</v>
+        <v>1235.95</v>
       </c>
       <c r="C4" t="n">
-        <v>798.1</v>
+        <v>747.788</v>
       </c>
       <c r="D4" t="n">
-        <v>757.15</v>
+        <v>747.1080000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>19-20</t>
+          <t>24-25</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>529.374</v>
+        <v>1362.52</v>
       </c>
       <c r="C5" t="n">
-        <v>545.8699999999999</v>
+        <v>1157.636</v>
       </c>
       <c r="D5" t="n">
-        <v>545.51</v>
+        <v>1157.036</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20-21</t>
+          <t>25-26</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>362.8</v>
+        <v>1572.957082855212</v>
       </c>
       <c r="C6" t="n">
-        <v>338.7</v>
+        <v>1652.044</v>
       </c>
       <c r="D6" t="n">
-        <v>306.6</v>
+        <v>1651.444</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>21-22</t>
+          <t>26-27</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>344.97</v>
+        <v>1124.88</v>
       </c>
       <c r="C7" t="n">
-        <v>432.4</v>
+        <v>1565.2</v>
       </c>
       <c r="D7" t="n">
-        <v>426.2</v>
+        <v>1564.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>22-23</t>
+          <t>27-28</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>943.0700000000001</v>
+        <v>534.5699999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>443.8</v>
+        <v>649.7239999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>443.2</v>
+        <v>649.124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>23-24</t>
+          <t>28-29</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1235.95</v>
+        <v>264.61</v>
       </c>
       <c r="C9" t="n">
-        <v>747.788</v>
+        <v>257.732</v>
       </c>
       <c r="D9" t="n">
-        <v>747.1080000000001</v>
+        <v>257.052</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>24-25</t>
+          <t>29-30</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1362.52</v>
+        <v>221.47</v>
       </c>
       <c r="C10" t="n">
-        <v>1157.636</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1157.036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>25-26</t>
+          <t>30-31</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1572.957082855212</v>
+        <v>223.66</v>
       </c>
       <c r="C11" t="n">
-        <v>1652.044</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1651.444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>26-27</t>
+          <t>31-32</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1124.88</v>
+        <v>226.79</v>
       </c>
       <c r="C12" t="n">
-        <v>1565.2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1564.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>27-28</t>
+          <t>32-33</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>534.5699999999999</v>
+        <v>229.96</v>
       </c>
       <c r="C13" t="n">
-        <v>649.7239999999999</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>649.124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>28-29</t>
+          <t>33-34</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>264.61</v>
+        <v>233.24</v>
       </c>
       <c r="C14" t="n">
-        <v>257.732</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>257.052</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>29-30</t>
+          <t>34-35</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>221.47</v>
+        <v>217.3</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -670,11 +670,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>30-31</t>
+          <t>35-36</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>223.66</v>
+        <v>145.94</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -686,11 +686,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>31-32</t>
+          <t>36-37</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>226.79</v>
+        <v>51.87</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -702,11 +702,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>32-33</t>
+          <t>37-38</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>229.96</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -718,11 +718,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>33-34</t>
+          <t>38-39</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>233.24</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -734,96 +734,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>34-35</t>
+          <t>39-40</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>217.3</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>35-36</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>145.94</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>36-37</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>51.87</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>37-38</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>38-39</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>39-40</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>